<commit_message>
RDM-4525 Fix Import definition integration test.
</commit_message>
<xml_diff>
--- a/application/src/test/resources/CCD_TestDefinition_V44_RDM-4525.xlsx
+++ b/application/src/test/resources/CCD_TestDefinition_V44_RDM-4525.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="29005"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohammedanaskhatri/definition-store/ccd-definition-store-api/application/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrzejfolga/src/ccd/temp/ccd-definition-store-api/application/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43FD6DD-4105-0B4B-88EB-C447C0BEC10B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19240" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14060" yWindow="-28340" windowWidth="51200" windowHeight="28340" tabRatio="500" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -1087,7 +1086,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd\/mm\/yyyy"/>
     <numFmt numFmtId="165" formatCode="d\/m\/yy"/>
@@ -1887,7 +1886,7 @@
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 2" xfId="7"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2315,7 +2314,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -2541,7 +2540,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2576,7 +2575,7 @@
       <c r="F1" s="99"/>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" spans="1:7" ht="70" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="65" x14ac:dyDescent="0.15">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="13" t="s">
@@ -2744,7 +2743,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2779,7 +2778,7 @@
       <c r="F1" s="60"/>
       <c r="G1" s="60"/>
     </row>
-    <row r="2" spans="1:7" ht="70" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="65" x14ac:dyDescent="0.15">
       <c r="A2" s="61"/>
       <c r="B2" s="61"/>
       <c r="C2" s="62" t="s">
@@ -3080,7 +3079,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3283,7 +3282,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
@@ -3331,7 +3330,7 @@
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
     </row>
-    <row r="2" spans="1:13" ht="70" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:13" ht="65" x14ac:dyDescent="0.15">
       <c r="A2" s="166"/>
       <c r="B2" s="166"/>
       <c r="C2" s="165" t="s">
@@ -3922,7 +3921,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
@@ -4120,8 +4119,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
-    <hyperlink ref="C5" r:id="rId2" xr:uid="{00000000-0004-0000-0D00-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId1"/>
+    <hyperlink ref="C5" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4132,7 +4131,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -4282,7 +4281,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IP12"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -7421,7 +7420,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -8023,7 +8022,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IU15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -12051,7 +12050,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IU15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -12935,7 +12934,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -13303,7 +13302,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13331,7 +13330,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="84" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="65" x14ac:dyDescent="0.15">
       <c r="A2" s="160"/>
       <c r="B2" s="160" t="s">
         <v>322</v>
@@ -13400,9 +13399,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-1300-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1">
           <x14:formula1>
-            <xm:f>'/Users/andrzejfolga/src/ccd/temp/ccd-definition-store-api/excel-importer/src/test/resources/[CCD_TestDefinition.xlsx]CaseType'!#REF!</xm:f>
+            <xm:f>[1]CaseType!#REF!</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
@@ -13416,7 +13415,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W42"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="D2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
@@ -14917,7 +14916,7 @@
       <c r="W42" s="37"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M32" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
+  <autoFilter ref="A1:M32"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
@@ -14927,7 +14926,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
@@ -15020,7 +15019,9 @@
       <c r="E4" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="F4" s="4"/>
+      <c r="F4" s="4">
+        <v>4</v>
+      </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -15040,7 +15041,9 @@
       <c r="E5" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="F5" s="4"/>
+      <c r="F5" s="4">
+        <v>2</v>
+      </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
@@ -15082,7 +15085,9 @@
       <c r="E7" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="F7" s="4"/>
+      <c r="F7" s="4">
+        <v>3</v>
+      </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -15278,7 +15283,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -16204,7 +16209,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -16584,7 +16589,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U19"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="150" workbookViewId="0">
@@ -17282,7 +17287,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
@@ -18072,7 +18077,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -18107,7 +18112,7 @@
       <c r="F1" s="177"/>
       <c r="G1" s="47"/>
     </row>
-    <row r="2" spans="1:7" ht="70" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="65" x14ac:dyDescent="0.15">
       <c r="A2" s="48"/>
       <c r="B2" s="48"/>
       <c r="C2" s="49" t="s">

</xml_diff>